<commit_message>
rm 2 US & add Native Son
</commit_message>
<xml_diff>
--- a/read_the_world.xlsx
+++ b/read_the_world.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682">
   <si>
     <t>Code</t>
   </si>
@@ -1906,28 +1906,16 @@
     <t>United States</t>
   </si>
   <si>
-    <t>The Color Purple</t>
-  </si>
-  <si>
-    <t>Alice Walker</t>
-  </si>
-  <si>
-    <t>Catcher in the Rye</t>
-  </si>
-  <si>
-    <t>J. D. Salinger</t>
+    <t>Native Son</t>
+  </si>
+  <si>
+    <t>Richard Wright</t>
   </si>
   <si>
     <t>To Kill a Mockingbird</t>
   </si>
   <si>
     <t>Harper Lee</t>
-  </si>
-  <si>
-    <t>Catch 22</t>
-  </si>
-  <si>
-    <t>Joseph Heller</t>
   </si>
   <si>
     <t>Parable of the Sower</t>
@@ -2079,9 +2067,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -2090,6 +2078,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2102,14 +2097,83 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2123,31 +2187,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2155,7 +2196,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2163,15 +2204,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2184,54 +2217,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2246,25 +2234,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2276,7 +2264,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2300,19 +2288,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2324,7 +2300,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2336,13 +2330,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2354,7 +2348,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2372,61 +2372,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2464,6 +2452,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2475,6 +2472,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2496,6 +2508,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2504,186 +2525,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3010,12 +2998,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F294"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G285" sqref="G285"/>
+      <selection pane="bottomLeft" activeCell="I275" sqref="I275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -6496,7 +6484,7 @@
         <v>631</v>
       </c>
       <c r="E269">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270" spans="1:5">
@@ -6535,36 +6523,24 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="B272" t="s">
-        <v>629</v>
-      </c>
-      <c r="C272" t="s">
-        <v>636</v>
-      </c>
-      <c r="D272" t="s">
         <v>637</v>
       </c>
       <c r="E272">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273" spans="1:5">
       <c r="A273" t="s">
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="B273" t="s">
-        <v>629</v>
-      </c>
-      <c r="C273" t="s">
-        <v>638</v>
-      </c>
-      <c r="D273" t="s">
         <v>639</v>
       </c>
       <c r="E273">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274" spans="1:5">
@@ -6706,16 +6682,28 @@
       <c r="B286" t="s">
         <v>665</v>
       </c>
+      <c r="C286" t="s">
+        <v>666</v>
+      </c>
+      <c r="D286" t="s">
+        <v>667</v>
+      </c>
       <c r="E286">
         <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:5">
       <c r="A287" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B287" t="s">
-        <v>667</v>
+        <v>665</v>
+      </c>
+      <c r="C287" t="s">
+        <v>668</v>
+      </c>
+      <c r="D287" t="s">
+        <v>669</v>
       </c>
       <c r="E287">
         <v>0</v>
@@ -6723,10 +6711,10 @@
     </row>
     <row r="288" spans="1:5">
       <c r="A288" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="B288" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C288" t="s">
         <v>670</v>
@@ -6735,20 +6723,14 @@
         <v>671</v>
       </c>
       <c r="E288">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:5">
       <c r="A289" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="B289" t="s">
-        <v>669</v>
-      </c>
-      <c r="C289" t="s">
-        <v>672</v>
-      </c>
-      <c r="D289" t="s">
         <v>673</v>
       </c>
       <c r="E289">
@@ -6757,27 +6739,33 @@
     </row>
     <row r="290" spans="1:5">
       <c r="A290" t="s">
-        <v>668</v>
+        <v>674</v>
       </c>
       <c r="B290" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
       <c r="C290" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="D290" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="E290">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:5">
       <c r="A291" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B291" t="s">
-        <v>677</v>
+        <v>675</v>
+      </c>
+      <c r="C291" t="s">
+        <v>678</v>
+      </c>
+      <c r="D291" t="s">
+        <v>679</v>
       </c>
       <c r="E291">
         <v>0</v>
@@ -6785,10 +6773,10 @@
     </row>
     <row r="292" spans="1:5">
       <c r="A292" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B292" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C292" t="s">
         <v>680</v>
@@ -6797,40 +6785,6 @@
         <v>681</v>
       </c>
       <c r="E292">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5">
-      <c r="A293" t="s">
-        <v>678</v>
-      </c>
-      <c r="B293" t="s">
-        <v>679</v>
-      </c>
-      <c r="C293" t="s">
-        <v>682</v>
-      </c>
-      <c r="D293" t="s">
-        <v>683</v>
-      </c>
-      <c r="E293">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="1:5">
-      <c r="A294" t="s">
-        <v>678</v>
-      </c>
-      <c r="B294" t="s">
-        <v>679</v>
-      </c>
-      <c r="C294" t="s">
-        <v>684</v>
-      </c>
-      <c r="D294" t="s">
-        <v>685</v>
-      </c>
-      <c r="E294">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Singapore and Czech Republic recommendations
</commit_message>
<xml_diff>
--- a/read_the_world.xlsx
+++ b/read_the_world.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$310</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$311</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751">
   <si>
     <t>Code</t>
   </si>
@@ -469,6 +469,15 @@
     <t>Milan Kundera</t>
   </si>
   <si>
+    <t>The Affliction of Praha</t>
+  </si>
+  <si>
+    <t>Simon Gillard</t>
+  </si>
+  <si>
+    <t>murder mystery set in 1920s Czechoslovakia</t>
+  </si>
+  <si>
     <t>CD</t>
   </si>
   <si>
@@ -1745,6 +1754,12 @@
   </si>
   <si>
     <t>Singapore</t>
+  </si>
+  <si>
+    <t>Kumar: From Rags to Drag</t>
+  </si>
+  <si>
+    <t>Kumarason "Kumar" Chinnadurai</t>
   </si>
   <si>
     <t>SX</t>
@@ -3201,12 +3216,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G310"/>
+  <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F196" sqref="F196"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -4033,63 +4048,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="s">
         <v>150</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>151</v>
       </c>
-      <c r="C65" t="s">
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
         <v>152</v>
-      </c>
-      <c r="D65" t="s">
-        <v>153</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B66" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C66" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D66" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B67" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C67" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D67" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B68" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" t="s">
         <v>159</v>
+      </c>
+      <c r="D68" t="s">
+        <v>160</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -4097,10 +4121,10 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -4108,10 +4132,10 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -4119,16 +4143,10 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B71" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" t="s">
         <v>166</v>
-      </c>
-      <c r="D71" t="s">
-        <v>167</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -4136,16 +4154,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
         <v>168</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>169</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>170</v>
-      </c>
-      <c r="D72" t="s">
-        <v>171</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -4153,10 +4171,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
+        <v>171</v>
+      </c>
+      <c r="B73" t="s">
         <v>172</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>173</v>
+      </c>
+      <c r="D73" t="s">
+        <v>174</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -4164,16 +4188,10 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B74" t="s">
-        <v>175</v>
-      </c>
-      <c r="C74" t="s">
         <v>176</v>
-      </c>
-      <c r="D74" t="s">
-        <v>177</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -4181,10 +4199,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
+        <v>177</v>
+      </c>
+      <c r="B75" t="s">
         <v>178</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>179</v>
+      </c>
+      <c r="D75" t="s">
+        <v>180</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -4192,10 +4216,10 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B76" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -4203,10 +4227,10 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B77" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -4214,10 +4238,10 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -4225,16 +4249,10 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B79" t="s">
-        <v>187</v>
-      </c>
-      <c r="C79" t="s">
         <v>188</v>
-      </c>
-      <c r="D79" t="s">
-        <v>189</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -4242,10 +4260,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
+        <v>189</v>
+      </c>
+      <c r="B80" t="s">
         <v>190</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>191</v>
+      </c>
+      <c r="D80" t="s">
+        <v>192</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -4253,16 +4277,10 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B81" t="s">
-        <v>193</v>
-      </c>
-      <c r="C81" t="s">
         <v>194</v>
-      </c>
-      <c r="D81" t="s">
-        <v>195</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -4270,10 +4288,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
+        <v>195</v>
+      </c>
+      <c r="B82" t="s">
         <v>196</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>197</v>
+      </c>
+      <c r="D82" t="s">
+        <v>198</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -4281,10 +4305,10 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B83" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -4292,16 +4316,10 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B84" t="s">
-        <v>201</v>
-      </c>
-      <c r="C84" t="s">
         <v>202</v>
-      </c>
-      <c r="D84" t="s">
-        <v>203</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -4309,16 +4327,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B85" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C85" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D85" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -4326,38 +4344,44 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B86" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C86" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D86" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B87" t="s">
+        <v>204</v>
+      </c>
+      <c r="C87" t="s">
         <v>209</v>
       </c>
+      <c r="D87" t="s">
+        <v>210</v>
+      </c>
       <c r="E87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B88" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -4365,10 +4389,10 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B89" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -4376,10 +4400,10 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B90" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -4387,10 +4411,10 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B91" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -4398,10 +4422,10 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B92" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -4409,33 +4433,27 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B93" t="s">
-        <v>221</v>
-      </c>
-      <c r="C93" t="s">
         <v>222</v>
       </c>
-      <c r="D93" t="s">
-        <v>223</v>
-      </c>
       <c r="E93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B94" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C94" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D94" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -4443,33 +4461,33 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B95" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C95" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D95" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B96" t="s">
+        <v>224</v>
+      </c>
+      <c r="C96" t="s">
         <v>229</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>230</v>
-      </c>
-      <c r="D96" t="s">
-        <v>231</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -4477,16 +4495,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B97" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C97" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D97" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -4494,16 +4512,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B98" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C98" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D98" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -4511,16 +4529,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B99" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C99" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D99" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -4528,44 +4546,44 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B100" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C100" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D100" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B101" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" t="s">
         <v>241</v>
       </c>
+      <c r="D101" t="s">
+        <v>242</v>
+      </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B102" t="s">
-        <v>243</v>
-      </c>
-      <c r="C102" t="s">
         <v>244</v>
-      </c>
-      <c r="D102" t="s">
-        <v>245</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -4573,16 +4591,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B103" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C103" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D103" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -4590,10 +4608,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B104" t="s">
+        <v>246</v>
+      </c>
+      <c r="C104" t="s">
         <v>249</v>
+      </c>
+      <c r="D104" t="s">
+        <v>250</v>
       </c>
       <c r="E104">
         <v>0</v>
@@ -4601,10 +4625,10 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B105" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E105">
         <v>0</v>
@@ -4612,10 +4636,10 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B106" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -4623,10 +4647,10 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B107" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -4634,10 +4658,10 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B108" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -4645,10 +4669,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B109" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E109">
         <v>0</v>
@@ -4656,38 +4680,38 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B110" t="s">
-        <v>261</v>
-      </c>
-      <c r="C110" t="s">
         <v>262</v>
       </c>
-      <c r="D110" t="s">
-        <v>263</v>
-      </c>
       <c r="E110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
+        <v>263</v>
+      </c>
+      <c r="B111" t="s">
         <v>264</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>265</v>
       </c>
+      <c r="D111" t="s">
+        <v>266</v>
+      </c>
       <c r="E111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B112" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E112">
         <v>0</v>
@@ -4695,16 +4719,10 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B113" t="s">
-        <v>269</v>
-      </c>
-      <c r="C113" t="s">
         <v>270</v>
-      </c>
-      <c r="D113" t="s">
-        <v>271</v>
       </c>
       <c r="E113">
         <v>0</v>
@@ -4712,10 +4730,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
+        <v>271</v>
+      </c>
+      <c r="B114" t="s">
         <v>272</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>273</v>
+      </c>
+      <c r="D114" t="s">
+        <v>274</v>
       </c>
       <c r="E114">
         <v>0</v>
@@ -4723,10 +4747,10 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B115" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E115">
         <v>0</v>
@@ -4734,10 +4758,10 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B116" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -4745,10 +4769,10 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B117" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -4756,50 +4780,44 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B118" t="s">
-        <v>281</v>
-      </c>
-      <c r="C118" t="s">
         <v>282</v>
       </c>
-      <c r="D118" t="s">
-        <v>283</v>
-      </c>
       <c r="E118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
+        <v>283</v>
+      </c>
+      <c r="B119" t="s">
         <v>284</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>285</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>286</v>
       </c>
-      <c r="D119" t="s">
-        <v>287</v>
-      </c>
       <c r="E119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B120" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C120" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D120" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -4807,16 +4825,16 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B121" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C121" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D121" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -4824,16 +4842,16 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B122" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C122" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D122" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -4841,89 +4859,89 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B123" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C123" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D123" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B124" t="s">
+        <v>288</v>
+      </c>
+      <c r="C124" t="s">
         <v>297</v>
       </c>
+      <c r="D124" t="s">
+        <v>298</v>
+      </c>
       <c r="E124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B125" t="s">
-        <v>299</v>
-      </c>
-      <c r="C125" t="s">
         <v>300</v>
       </c>
-      <c r="D125" t="s">
-        <v>301</v>
-      </c>
       <c r="E125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
+        <v>301</v>
+      </c>
+      <c r="B126" t="s">
         <v>302</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>303</v>
       </c>
+      <c r="D126" t="s">
+        <v>304</v>
+      </c>
       <c r="E126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B127" t="s">
-        <v>305</v>
-      </c>
-      <c r="C127" t="s">
         <v>306</v>
       </c>
-      <c r="D127" t="s">
-        <v>307</v>
-      </c>
       <c r="E127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B128" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C128" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D128" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -4931,58 +4949,55 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="B129" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C129" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D129" t="s">
         <v>310</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B130" t="s">
+        <v>308</v>
+      </c>
+      <c r="C130" t="s">
         <v>312</v>
       </c>
+      <c r="D130" t="s">
+        <v>313</v>
+      </c>
       <c r="E130">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B131" t="s">
-        <v>314</v>
-      </c>
-      <c r="C131" t="s">
         <v>315</v>
       </c>
-      <c r="D131" t="s">
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" t="s">
         <v>316</v>
       </c>
-      <c r="E131">
-        <v>0</v>
-      </c>
-      <c r="F131" t="s">
+      <c r="B132" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
-      <c r="A132" t="s">
-        <v>313</v>
-      </c>
-      <c r="B132" t="s">
-        <v>314</v>
       </c>
       <c r="C132" t="s">
         <v>318</v>
@@ -4993,19 +5008,22 @@
       <c r="E132">
         <v>0</v>
       </c>
+      <c r="F132" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B133" t="s">
+        <v>317</v>
+      </c>
+      <c r="C133" t="s">
         <v>321</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>322</v>
-      </c>
-      <c r="D133" t="s">
-        <v>323</v>
       </c>
       <c r="E133">
         <v>0</v>
@@ -5013,10 +5031,16 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" t="s">
+        <v>323</v>
+      </c>
+      <c r="B134" t="s">
         <v>324</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>325</v>
+      </c>
+      <c r="D134" t="s">
+        <v>326</v>
       </c>
       <c r="E134">
         <v>0</v>
@@ -5024,10 +5048,10 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B135" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E135">
         <v>0</v>
@@ -5035,16 +5059,10 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B136" t="s">
-        <v>329</v>
-      </c>
-      <c r="C136" t="s">
         <v>330</v>
-      </c>
-      <c r="D136" t="s">
-        <v>331</v>
       </c>
       <c r="E136">
         <v>0</v>
@@ -5052,33 +5070,33 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B137" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C137" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D137" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E137">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B138" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="C138" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D138" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -5086,21 +5104,27 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B139" t="s">
+        <v>332</v>
+      </c>
+      <c r="C139" t="s">
         <v>337</v>
       </c>
+      <c r="D139" t="s">
+        <v>338</v>
+      </c>
       <c r="E139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B140" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -5108,10 +5132,10 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B141" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E141">
         <v>0</v>
@@ -5119,16 +5143,10 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B142" t="s">
-        <v>343</v>
-      </c>
-      <c r="C142" t="s">
         <v>344</v>
-      </c>
-      <c r="D142" t="s">
-        <v>345</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -5136,16 +5154,16 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B143" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C143" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D143" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -5153,33 +5171,33 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B144" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C144" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D144" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B145" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C145" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D145" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -5187,16 +5205,16 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B146" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C146" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D146" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E146">
         <v>1</v>
@@ -5204,21 +5222,27 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="B147" t="s">
+        <v>346</v>
+      </c>
+      <c r="C147" t="s">
         <v>355</v>
       </c>
+      <c r="D147" t="s">
+        <v>356</v>
+      </c>
       <c r="E147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B148" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E148">
         <v>0</v>
@@ -5226,10 +5250,10 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B149" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E149">
         <v>0</v>
@@ -5237,10 +5261,10 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B150" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E150">
         <v>0</v>
@@ -5248,10 +5272,10 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B151" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E151">
         <v>0</v>
@@ -5259,73 +5283,73 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B152" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E152">
         <v>0</v>
       </c>
     </row>
-    <row r="153" ht="16.8" spans="1:7">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B153" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E153">
         <v>0</v>
       </c>
-      <c r="G153" s="1"/>
     </row>
     <row r="154" ht="16.8" spans="1:7">
       <c r="A154" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B154" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E154">
         <v>0</v>
       </c>
       <c r="G154" s="1"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" ht="16.8" spans="1:7">
       <c r="A155" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B155" t="s">
-        <v>371</v>
-      </c>
-      <c r="C155" t="s">
         <v>372</v>
       </c>
-      <c r="D155" t="s">
-        <v>373</v>
-      </c>
       <c r="E155">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G155" s="1"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" t="s">
+        <v>373</v>
+      </c>
+      <c r="B156" t="s">
         <v>374</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" t="s">
         <v>375</v>
       </c>
+      <c r="D156" t="s">
+        <v>376</v>
+      </c>
       <c r="E156">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B157" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E157">
         <v>0</v>
@@ -5333,10 +5357,10 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B158" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E158">
         <v>0</v>
@@ -5344,10 +5368,10 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B159" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E159">
         <v>0</v>
@@ -5355,10 +5379,10 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B160" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E160">
         <v>0</v>
@@ -5366,10 +5390,10 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B161" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E161">
         <v>0</v>
@@ -5377,10 +5401,10 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B162" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E162">
         <v>0</v>
@@ -5388,10 +5412,10 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B163" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E163">
         <v>0</v>
@@ -5399,33 +5423,27 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B164" t="s">
-        <v>391</v>
-      </c>
-      <c r="C164" t="s">
         <v>392</v>
       </c>
-      <c r="D164" t="s">
-        <v>393</v>
-      </c>
       <c r="E164">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B165" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C165" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D165" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E165">
         <v>1</v>
@@ -5433,69 +5451,75 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B166" t="s">
+        <v>394</v>
+      </c>
+      <c r="C166" t="s">
+        <v>397</v>
+      </c>
+      <c r="D166" t="s">
         <v>396</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B167" t="s">
-        <v>398</v>
-      </c>
-      <c r="C167" t="s">
         <v>399</v>
       </c>
-      <c r="D167" t="s">
+      <c r="E167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
         <v>400</v>
       </c>
-      <c r="E167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" t="s">
-        <v>397</v>
-      </c>
       <c r="B168" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C168" t="s">
+        <v>402</v>
+      </c>
+      <c r="D168" t="s">
+        <v>403</v>
+      </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" t="s">
+        <v>400</v>
+      </c>
+      <c r="B169" t="s">
         <v>401</v>
       </c>
-      <c r="D168" t="s">
-        <v>402</v>
-      </c>
-      <c r="E168">
+      <c r="C169" t="s">
+        <v>404</v>
+      </c>
+      <c r="D169" t="s">
+        <v>405</v>
+      </c>
+      <c r="E169">
         <v>1</v>
       </c>
-      <c r="F168" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5">
-      <c r="A169" t="s">
-        <v>404</v>
-      </c>
-      <c r="B169" t="s">
-        <v>405</v>
-      </c>
-      <c r="E169">
-        <v>0</v>
+      <c r="F169" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="170" spans="1:5">
       <c r="A170" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B170" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E170">
         <v>0</v>
@@ -5503,10 +5527,10 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B171" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E171">
         <v>0</v>
@@ -5514,10 +5538,10 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B172" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E172">
         <v>0</v>
@@ -5525,10 +5549,10 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B173" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E173">
         <v>0</v>
@@ -5536,10 +5560,10 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B174" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E174">
         <v>0</v>
@@ -5547,38 +5571,38 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B175" t="s">
-        <v>417</v>
-      </c>
-      <c r="C175" t="s">
         <v>418</v>
       </c>
-      <c r="D175" t="s">
-        <v>419</v>
-      </c>
       <c r="E175">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" t="s">
+        <v>419</v>
+      </c>
+      <c r="B176" t="s">
         <v>420</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
         <v>421</v>
       </c>
+      <c r="D176" t="s">
+        <v>422</v>
+      </c>
       <c r="E176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B177" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E177">
         <v>0</v>
@@ -5586,10 +5610,10 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B178" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E178">
         <v>0</v>
@@ -5597,10 +5621,10 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B179" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E179">
         <v>0</v>
@@ -5608,10 +5632,10 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B180" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E180">
         <v>0</v>
@@ -5619,10 +5643,10 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B181" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E181">
         <v>0</v>
@@ -5630,10 +5654,10 @@
     </row>
     <row r="182" spans="1:5">
       <c r="A182" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B182" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E182">
         <v>0</v>
@@ -5641,16 +5665,10 @@
     </row>
     <row r="183" spans="1:5">
       <c r="A183" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B183" t="s">
-        <v>435</v>
-      </c>
-      <c r="C183" t="s">
         <v>436</v>
-      </c>
-      <c r="D183" t="s">
-        <v>437</v>
       </c>
       <c r="E183">
         <v>0</v>
@@ -5658,10 +5676,16 @@
     </row>
     <row r="184" spans="1:5">
       <c r="A184" t="s">
+        <v>437</v>
+      </c>
+      <c r="B184" t="s">
         <v>438</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C184" t="s">
         <v>439</v>
+      </c>
+      <c r="D184" t="s">
+        <v>440</v>
       </c>
       <c r="E184">
         <v>0</v>
@@ -5669,10 +5693,10 @@
     </row>
     <row r="185" spans="1:5">
       <c r="A185" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B185" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E185">
         <v>0</v>
@@ -5680,10 +5704,10 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B186" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E186">
         <v>0</v>
@@ -5691,10 +5715,10 @@
     </row>
     <row r="187" spans="1:5">
       <c r="A187" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B187" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E187">
         <v>0</v>
@@ -5702,38 +5726,38 @@
     </row>
     <row r="188" spans="1:5">
       <c r="A188" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B188" t="s">
-        <v>447</v>
-      </c>
-      <c r="C188" t="s">
         <v>448</v>
       </c>
-      <c r="D188" t="s">
-        <v>449</v>
-      </c>
       <c r="E188">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" t="s">
+        <v>449</v>
+      </c>
+      <c r="B189" t="s">
         <v>450</v>
       </c>
-      <c r="B189" t="s">
+      <c r="C189" t="s">
         <v>451</v>
       </c>
+      <c r="D189" t="s">
+        <v>452</v>
+      </c>
       <c r="E189">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:5">
       <c r="A190" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B190" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E190">
         <v>0</v>
@@ -5741,10 +5765,10 @@
     </row>
     <row r="191" spans="1:5">
       <c r="A191" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B191" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E191">
         <v>0</v>
@@ -5752,10 +5776,10 @@
     </row>
     <row r="192" spans="1:5">
       <c r="A192" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B192" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E192">
         <v>0</v>
@@ -5763,64 +5787,55 @@
     </row>
     <row r="193" spans="1:5">
       <c r="A193" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B193" t="s">
-        <v>459</v>
-      </c>
-      <c r="C193" t="s">
         <v>460</v>
       </c>
-      <c r="D193" t="s">
-        <v>461</v>
-      </c>
       <c r="E193">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B194" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C194" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D194" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E194">
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B195" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C195" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D195" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E195">
-        <v>0</v>
-      </c>
-      <c r="F195" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="B196" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C196" t="s">
         <v>467</v>
@@ -5831,13 +5846,22 @@
       <c r="E196">
         <v>0</v>
       </c>
+      <c r="F196" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="B197" t="s">
+        <v>462</v>
+      </c>
+      <c r="C197" t="s">
         <v>470</v>
+      </c>
+      <c r="D197" t="s">
+        <v>471</v>
       </c>
       <c r="E197">
         <v>0</v>
@@ -5845,10 +5869,10 @@
     </row>
     <row r="198" spans="1:5">
       <c r="A198" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B198" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E198">
         <v>0</v>
@@ -5856,16 +5880,10 @@
     </row>
     <row r="199" spans="1:5">
       <c r="A199" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B199" t="s">
-        <v>474</v>
-      </c>
-      <c r="C199" t="s">
         <v>475</v>
-      </c>
-      <c r="D199" t="s">
-        <v>476</v>
       </c>
       <c r="E199">
         <v>0</v>
@@ -5873,10 +5891,16 @@
     </row>
     <row r="200" spans="1:5">
       <c r="A200" t="s">
+        <v>476</v>
+      </c>
+      <c r="B200" t="s">
         <v>477</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
         <v>478</v>
+      </c>
+      <c r="D200" t="s">
+        <v>479</v>
       </c>
       <c r="E200">
         <v>0</v>
@@ -5884,16 +5908,10 @@
     </row>
     <row r="201" spans="1:5">
       <c r="A201" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B201" t="s">
-        <v>480</v>
-      </c>
-      <c r="C201" t="s">
         <v>481</v>
-      </c>
-      <c r="D201" t="s">
-        <v>482</v>
       </c>
       <c r="E201">
         <v>0</v>
@@ -5901,16 +5919,16 @@
     </row>
     <row r="202" spans="1:5">
       <c r="A202" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B202" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C202" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D202" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="E202">
         <v>0</v>
@@ -5918,52 +5936,58 @@
     </row>
     <row r="203" spans="1:5">
       <c r="A203" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B203" t="s">
+        <v>483</v>
+      </c>
+      <c r="C203" t="s">
+        <v>486</v>
+      </c>
+      <c r="D203" t="s">
         <v>485</v>
       </c>
       <c r="E203">
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B204" t="s">
-        <v>487</v>
-      </c>
-      <c r="C204" t="s">
         <v>488</v>
       </c>
-      <c r="D204" t="s">
+      <c r="E204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" t="s">
         <v>489</v>
       </c>
-      <c r="E204">
-        <v>0</v>
-      </c>
-      <c r="F204" t="s">
+      <c r="B205" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="205" spans="1:5">
-      <c r="A205" t="s">
+      <c r="C205" t="s">
         <v>491</v>
       </c>
-      <c r="B205" t="s">
+      <c r="D205" t="s">
         <v>492</v>
       </c>
       <c r="E205">
         <v>0</v>
+      </c>
+      <c r="F205" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="206" spans="1:5">
       <c r="A206" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B206" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="E206">
         <v>0</v>
@@ -5971,10 +5995,10 @@
     </row>
     <row r="207" spans="1:5">
       <c r="A207" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B207" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E207">
         <v>0</v>
@@ -5982,16 +6006,10 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B208" t="s">
-        <v>498</v>
-      </c>
-      <c r="C208" t="s">
         <v>499</v>
-      </c>
-      <c r="D208" t="s">
-        <v>500</v>
       </c>
       <c r="E208">
         <v>0</v>
@@ -5999,10 +6017,16 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" t="s">
+        <v>500</v>
+      </c>
+      <c r="B209" t="s">
         <v>501</v>
       </c>
-      <c r="B209" t="s">
+      <c r="C209" t="s">
         <v>502</v>
+      </c>
+      <c r="D209" t="s">
+        <v>503</v>
       </c>
       <c r="E209">
         <v>0</v>
@@ -6010,38 +6034,38 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B210" t="s">
-        <v>504</v>
-      </c>
-      <c r="C210" t="s">
         <v>505</v>
       </c>
-      <c r="D210" t="s">
-        <v>506</v>
-      </c>
       <c r="E210">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
+        <v>506</v>
+      </c>
+      <c r="B211" t="s">
         <v>507</v>
       </c>
-      <c r="B211" t="s">
+      <c r="C211" t="s">
         <v>508</v>
       </c>
+      <c r="D211" t="s">
+        <v>509</v>
+      </c>
       <c r="E211">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B212" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E212">
         <v>0</v>
@@ -6049,16 +6073,10 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B213" t="s">
-        <v>512</v>
-      </c>
-      <c r="C213" t="s">
         <v>513</v>
-      </c>
-      <c r="D213" t="s">
-        <v>514</v>
       </c>
       <c r="E213">
         <v>0</v>
@@ -6066,38 +6084,44 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="B214" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="C214" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D214" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E214">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:5">
       <c r="A215" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B215" t="s">
+        <v>515</v>
+      </c>
+      <c r="C215" t="s">
         <v>518</v>
       </c>
+      <c r="D215" t="s">
+        <v>519</v>
+      </c>
       <c r="E215">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:5">
       <c r="A216" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B216" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E216">
         <v>0</v>
@@ -6105,10 +6129,10 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B217" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E217">
         <v>0</v>
@@ -6116,10 +6140,10 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B218" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E218">
         <v>0</v>
@@ -6127,10 +6151,10 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B219" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E219">
         <v>0</v>
@@ -6138,16 +6162,10 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B220" t="s">
-        <v>528</v>
-      </c>
-      <c r="C220" t="s">
         <v>529</v>
-      </c>
-      <c r="D220" t="s">
-        <v>530</v>
       </c>
       <c r="E220">
         <v>0</v>
@@ -6155,16 +6173,16 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B221" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C221" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D221" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E221">
         <v>0</v>
@@ -6172,16 +6190,16 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B222" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C222" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D222" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E222">
         <v>0</v>
@@ -6189,44 +6207,50 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B223" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C223" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D223" t="s">
-        <v>207</v>
+        <v>537</v>
       </c>
       <c r="E223">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:5">
       <c r="A224" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="B224" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="C224" t="s">
         <v>538</v>
       </c>
       <c r="D224" t="s">
-        <v>539</v>
+        <v>210</v>
       </c>
       <c r="E224">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:5">
       <c r="A225" t="s">
+        <v>539</v>
+      </c>
+      <c r="B225" t="s">
         <v>540</v>
       </c>
-      <c r="B225" t="s">
+      <c r="C225" t="s">
         <v>541</v>
+      </c>
+      <c r="D225" t="s">
+        <v>542</v>
       </c>
       <c r="E225">
         <v>0</v>
@@ -6234,10 +6258,10 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B226" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E226">
         <v>0</v>
@@ -6245,10 +6269,10 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B227" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E227">
         <v>0</v>
@@ -6256,10 +6280,10 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B228" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E228">
         <v>0</v>
@@ -6267,10 +6291,10 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B229" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E229">
         <v>0</v>
@@ -6278,10 +6302,10 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B230" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E230">
         <v>0</v>
@@ -6289,10 +6313,10 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B231" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E231">
         <v>0</v>
@@ -6300,10 +6324,10 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B232" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E232">
         <v>0</v>
@@ -6311,10 +6335,10 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B233" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E233">
         <v>0</v>
@@ -6322,10 +6346,10 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B234" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E234">
         <v>0</v>
@@ -6333,10 +6357,10 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B235" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E235">
         <v>0</v>
@@ -6344,16 +6368,10 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B236" t="s">
-        <v>563</v>
-      </c>
-      <c r="C236" t="s">
         <v>564</v>
-      </c>
-      <c r="D236" t="s">
-        <v>565</v>
       </c>
       <c r="E236">
         <v>0</v>
@@ -6361,10 +6379,16 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" t="s">
+        <v>565</v>
+      </c>
+      <c r="B237" t="s">
         <v>566</v>
       </c>
-      <c r="B237" t="s">
+      <c r="C237" t="s">
         <v>567</v>
+      </c>
+      <c r="D237" t="s">
+        <v>568</v>
       </c>
       <c r="E237">
         <v>0</v>
@@ -6372,10 +6396,10 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B238" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E238">
         <v>0</v>
@@ -6383,16 +6407,10 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B239" t="s">
-        <v>571</v>
-      </c>
-      <c r="C239" t="s">
         <v>572</v>
-      </c>
-      <c r="D239" t="s">
-        <v>573</v>
       </c>
       <c r="E239">
         <v>0</v>
@@ -6400,10 +6418,16 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" t="s">
+        <v>573</v>
+      </c>
+      <c r="B240" t="s">
         <v>574</v>
       </c>
-      <c r="B240" t="s">
+      <c r="C240" t="s">
         <v>575</v>
+      </c>
+      <c r="D240" t="s">
+        <v>576</v>
       </c>
       <c r="E240">
         <v>0</v>
@@ -6411,10 +6435,16 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B241" t="s">
-        <v>577</v>
+        <v>578</v>
+      </c>
+      <c r="C241" t="s">
+        <v>579</v>
+      </c>
+      <c r="D241" t="s">
+        <v>580</v>
       </c>
       <c r="E241">
         <v>0</v>
@@ -6422,10 +6452,10 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="B242" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="E242">
         <v>0</v>
@@ -6433,10 +6463,10 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="B243" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="E243">
         <v>0</v>
@@ -6444,10 +6474,10 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="B244" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="E244">
         <v>0</v>
@@ -6455,16 +6485,10 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="B245" t="s">
-        <v>585</v>
-      </c>
-      <c r="C245" t="s">
-        <v>586</v>
-      </c>
-      <c r="D245" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="E245">
         <v>0</v>
@@ -6472,16 +6496,16 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="B246" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="C246" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="D246" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="E246">
         <v>0</v>
@@ -6489,16 +6513,16 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" t="s">
+        <v>589</v>
+      </c>
+      <c r="B247" t="s">
         <v>590</v>
       </c>
-      <c r="B247" t="s">
-        <v>591</v>
-      </c>
       <c r="C247" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D247" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E247">
         <v>0</v>
@@ -6506,16 +6530,16 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B248" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="C248" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="D248" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="E248">
         <v>0</v>
@@ -6523,38 +6547,44 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B249" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="C249" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="D249" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="E249">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:5">
       <c r="A250" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B250" t="s">
-        <v>599</v>
+        <v>596</v>
+      </c>
+      <c r="C250" t="s">
+        <v>601</v>
+      </c>
+      <c r="D250" t="s">
+        <v>602</v>
       </c>
       <c r="E250">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:5">
       <c r="A251" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="B251" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="E251">
         <v>0</v>
@@ -6562,16 +6592,10 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="B252" t="s">
-        <v>603</v>
-      </c>
-      <c r="C252" t="s">
-        <v>604</v>
-      </c>
-      <c r="D252" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="E252">
         <v>0</v>
@@ -6579,16 +6603,16 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B253" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C253" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D253" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E253">
         <v>0</v>
@@ -6596,16 +6620,16 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="B254" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="C254" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="D254" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="E254">
         <v>0</v>
@@ -6613,16 +6637,16 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="B255" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="C255" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="D255" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="E255">
         <v>0</v>
@@ -6630,16 +6654,16 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="B256" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="C256" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="D256" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="E256">
         <v>0</v>
@@ -6647,16 +6671,16 @@
     </row>
     <row r="257" spans="1:5">
       <c r="A257" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="B257" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="C257" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="D257" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="E257">
         <v>0</v>
@@ -6664,16 +6688,16 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="B258" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="C258" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="D258" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="E258">
         <v>0</v>
@@ -6681,10 +6705,16 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
       <c r="B259" t="s">
-        <v>621</v>
+        <v>612</v>
+      </c>
+      <c r="C259" t="s">
+        <v>623</v>
+      </c>
+      <c r="D259" t="s">
+        <v>624</v>
       </c>
       <c r="E259">
         <v>0</v>
@@ -6692,16 +6722,10 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="B260" t="s">
-        <v>623</v>
-      </c>
-      <c r="C260" t="s">
-        <v>624</v>
-      </c>
-      <c r="D260" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E260">
         <v>0</v>
@@ -6709,10 +6733,16 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B261" t="s">
-        <v>627</v>
+        <v>628</v>
+      </c>
+      <c r="C261" t="s">
+        <v>629</v>
+      </c>
+      <c r="D261" t="s">
+        <v>630</v>
       </c>
       <c r="E261">
         <v>0</v>
@@ -6720,10 +6750,10 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="B262" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="E262">
         <v>0</v>
@@ -6731,10 +6761,10 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="B263" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="E263">
         <v>0</v>
@@ -6742,16 +6772,10 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="B264" t="s">
-        <v>633</v>
-      </c>
-      <c r="C264" t="s">
-        <v>634</v>
-      </c>
-      <c r="D264" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="E264">
         <v>0</v>
@@ -6759,16 +6783,16 @@
     </row>
     <row r="265" spans="1:5">
       <c r="A265" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="B265" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="C265" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="D265" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="E265">
         <v>0</v>
@@ -6782,7 +6806,7 @@
         <v>638</v>
       </c>
       <c r="C266" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D266" t="s">
         <v>640</v>
@@ -6793,16 +6817,16 @@
     </row>
     <row r="267" spans="1:5">
       <c r="A267" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="B267" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="C267" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="D267" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="E267">
         <v>0</v>
@@ -6810,16 +6834,16 @@
     </row>
     <row r="268" spans="1:5">
       <c r="A268" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="B268" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="C268" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="D268" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="E268">
         <v>0</v>
@@ -6827,13 +6851,13 @@
     </row>
     <row r="269" spans="1:5">
       <c r="A269" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B269" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C269" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="D269" t="s">
         <v>647</v>
@@ -6844,10 +6868,16 @@
     </row>
     <row r="270" spans="1:5">
       <c r="A270" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B270" t="s">
-        <v>649</v>
+        <v>650</v>
+      </c>
+      <c r="C270" t="s">
+        <v>651</v>
+      </c>
+      <c r="D270" t="s">
+        <v>652</v>
       </c>
       <c r="E270">
         <v>0</v>
@@ -6855,10 +6885,10 @@
     </row>
     <row r="271" spans="1:5">
       <c r="A271" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="B271" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="E271">
         <v>0</v>
@@ -6866,10 +6896,10 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="B272" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="E272">
         <v>0</v>
@@ -6877,16 +6907,10 @@
     </row>
     <row r="273" spans="1:5">
       <c r="A273" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="B273" t="s">
-        <v>655</v>
-      </c>
-      <c r="C273" t="s">
-        <v>656</v>
-      </c>
-      <c r="D273" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E273">
         <v>0</v>
@@ -6894,16 +6918,16 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="B274" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C274" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="D274" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
       <c r="E274">
         <v>0</v>
@@ -6911,16 +6935,16 @@
     </row>
     <row r="275" spans="1:5">
       <c r="A275" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="B275" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
       <c r="C275" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="D275" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="E275">
         <v>0</v>
@@ -6928,10 +6952,16 @@
     </row>
     <row r="276" spans="1:5">
       <c r="A276" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B276" t="s">
-        <v>662</v>
+        <v>660</v>
+      </c>
+      <c r="C276" t="s">
+        <v>664</v>
+      </c>
+      <c r="D276" t="s">
+        <v>665</v>
       </c>
       <c r="E276">
         <v>0</v>
@@ -6939,10 +6969,10 @@
     </row>
     <row r="277" spans="1:5">
       <c r="A277" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="B277" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="E277">
         <v>0</v>
@@ -6950,10 +6980,10 @@
     </row>
     <row r="278" spans="1:5">
       <c r="A278" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="B278" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="E278">
         <v>0</v>
@@ -6961,10 +6991,10 @@
     </row>
     <row r="279" spans="1:5">
       <c r="A279" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="B279" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="E279">
         <v>0</v>
@@ -6972,44 +7002,38 @@
     </row>
     <row r="280" spans="1:5">
       <c r="A280" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="B280" t="s">
-        <v>670</v>
-      </c>
-      <c r="C280" t="s">
-        <v>671</v>
-      </c>
-      <c r="D280" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E280">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:5">
       <c r="A281" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B281" t="s">
-        <v>674</v>
+        <v>675</v>
+      </c>
+      <c r="C281" t="s">
+        <v>676</v>
+      </c>
+      <c r="D281" t="s">
+        <v>677</v>
       </c>
       <c r="E281">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282" spans="1:5">
       <c r="A282" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="B282" t="s">
-        <v>676</v>
-      </c>
-      <c r="C282" t="s">
-        <v>677</v>
-      </c>
-      <c r="D282" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E282">
         <v>0</v>
@@ -7017,16 +7041,16 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
       <c r="B283" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="C283" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="D283" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="E283">
         <v>0</v>
@@ -7034,10 +7058,16 @@
     </row>
     <row r="284" spans="1:5">
       <c r="A284" t="s">
+        <v>680</v>
+      </c>
+      <c r="B284" t="s">
         <v>681</v>
       </c>
-      <c r="B284" t="s">
-        <v>682</v>
+      <c r="C284" t="s">
+        <v>684</v>
+      </c>
+      <c r="D284" t="s">
+        <v>685</v>
       </c>
       <c r="E284">
         <v>0</v>
@@ -7045,10 +7075,10 @@
     </row>
     <row r="285" spans="1:5">
       <c r="A285" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B285" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="E285">
         <v>0</v>
@@ -7056,10 +7086,10 @@
     </row>
     <row r="286" spans="1:5">
       <c r="A286" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="B286" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="E286">
         <v>0</v>
@@ -7067,10 +7097,10 @@
     </row>
     <row r="287" spans="1:5">
       <c r="A287" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="B287" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="E287">
         <v>0</v>
@@ -7078,10 +7108,10 @@
     </row>
     <row r="288" spans="1:5">
       <c r="A288" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="B288" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="E288">
         <v>0</v>
@@ -7089,44 +7119,44 @@
     </row>
     <row r="289" spans="1:5">
       <c r="A289" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="B289" t="s">
-        <v>692</v>
-      </c>
-      <c r="C289" t="s">
-        <v>693</v>
-      </c>
-      <c r="D289" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E289">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="290" spans="1:5">
       <c r="A290" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B290" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C290" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D290" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="E290">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="291" spans="1:5">
       <c r="A291" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B291" t="s">
-        <v>700</v>
+        <v>701</v>
+      </c>
+      <c r="C291" t="s">
+        <v>702</v>
+      </c>
+      <c r="D291" t="s">
+        <v>703</v>
       </c>
       <c r="E291">
         <v>0</v>
@@ -7134,10 +7164,10 @@
     </row>
     <row r="292" spans="1:5">
       <c r="A292" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="B292" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="E292">
         <v>0</v>
@@ -7145,33 +7175,27 @@
     </row>
     <row r="293" spans="1:5">
       <c r="A293" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="B293" t="s">
-        <v>704</v>
-      </c>
-      <c r="C293" t="s">
-        <v>705</v>
-      </c>
-      <c r="D293" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="E293">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:5">
       <c r="A294" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="B294" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
       <c r="C294" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="D294" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="E294">
         <v>1</v>
@@ -7179,16 +7203,16 @@
     </row>
     <row r="295" spans="1:5">
       <c r="A295" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="B295" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
       <c r="C295" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="D295" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="E295">
         <v>1</v>
@@ -7196,16 +7220,16 @@
     </row>
     <row r="296" spans="1:5">
       <c r="A296" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="B296" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
       <c r="C296" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="D296" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="E296">
         <v>1</v>
@@ -7213,21 +7237,27 @@
     </row>
     <row r="297" spans="1:5">
       <c r="A297" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="B297" t="s">
-        <v>714</v>
+        <v>709</v>
+      </c>
+      <c r="C297" t="s">
+        <v>716</v>
+      </c>
+      <c r="D297" t="s">
+        <v>717</v>
       </c>
       <c r="E297">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="298" spans="1:5">
       <c r="A298" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="B298" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="E298">
         <v>0</v>
@@ -7235,10 +7265,10 @@
     </row>
     <row r="299" spans="1:5">
       <c r="A299" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="B299" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="E299">
         <v>0</v>
@@ -7246,10 +7276,10 @@
     </row>
     <row r="300" spans="1:5">
       <c r="A300" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B300" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="E300">
         <v>0</v>
@@ -7257,52 +7287,52 @@
     </row>
     <row r="301" spans="1:5">
       <c r="A301" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B301" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="E301">
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:6">
+    <row r="302" spans="1:5">
       <c r="A302" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
       <c r="B302" t="s">
-        <v>724</v>
-      </c>
-      <c r="C302" t="s">
-        <v>725</v>
-      </c>
-      <c r="D302" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="E302">
-        <v>1</v>
-      </c>
-      <c r="F302" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="303" spans="1:5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6">
       <c r="A303" t="s">
         <v>728</v>
       </c>
       <c r="B303" t="s">
         <v>729</v>
       </c>
+      <c r="C303" t="s">
+        <v>730</v>
+      </c>
+      <c r="D303" t="s">
+        <v>731</v>
+      </c>
       <c r="E303">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F303" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="304" spans="1:5">
       <c r="A304" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="B304" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="E304">
         <v>0</v>
@@ -7310,10 +7340,10 @@
     </row>
     <row r="305" spans="1:5">
       <c r="A305" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="B305" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="E305">
         <v>0</v>
@@ -7321,10 +7351,10 @@
     </row>
     <row r="306" spans="1:5">
       <c r="A306" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="B306" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="E306">
         <v>0</v>
@@ -7332,16 +7362,10 @@
     </row>
     <row r="307" spans="1:5">
       <c r="A307" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="B307" t="s">
-        <v>737</v>
-      </c>
-      <c r="C307" t="s">
-        <v>738</v>
-      </c>
-      <c r="D307" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="E307">
         <v>0</v>
@@ -7349,16 +7373,16 @@
     </row>
     <row r="308" spans="1:5">
       <c r="A308" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
       <c r="B308" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="C308" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="D308" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="E308">
         <v>0</v>
@@ -7366,16 +7390,16 @@
     </row>
     <row r="309" spans="1:5">
       <c r="A309" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
       <c r="B309" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="C309" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="D309" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="E309">
         <v>0</v>
@@ -7383,18 +7407,35 @@
     </row>
     <row r="310" spans="1:5">
       <c r="A310" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="B310" t="s">
-        <v>745</v>
+        <v>742</v>
+      </c>
+      <c r="C310" t="s">
+        <v>747</v>
+      </c>
+      <c r="D310" t="s">
+        <v>748</v>
       </c>
       <c r="E310">
         <v>0</v>
       </c>
     </row>
+    <row r="311" spans="1:5">
+      <c r="A311" t="s">
+        <v>749</v>
+      </c>
+      <c r="B311" t="s">
+        <v>750</v>
+      </c>
+      <c r="E311">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F310">
-    <sortState ref="A2:F310">
+  <autoFilter ref="A1:F311">
+    <sortState ref="A2:F311">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
add Norwegian book Mayor Pete likes see also https://web.archive.org/web/20190317010614/https://twitter.com/AnandWrites/status/1106955561248149510
</commit_message>
<xml_diff>
--- a/read_the_world.xlsx
+++ b/read_the_world.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$311</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$312</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754">
   <si>
     <t>Code</t>
   </si>
@@ -1478,6 +1478,15 @@
   </si>
   <si>
     <t>Through a Glass, Darkly</t>
+  </si>
+  <si>
+    <t>Naïve. Super</t>
+  </si>
+  <si>
+    <t>Erlend Loe</t>
+  </si>
+  <si>
+    <t>book that inspired Mayor Pete to learn Norwegian (https://www.newyorker.com/books/page-turner/the-coming-of-age-tale-that-inspired-mayor-pete-to-learn-norwegian)</t>
   </si>
   <si>
     <t>OM</t>
@@ -3216,12 +3225,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G311"/>
+  <dimension ref="A1:G312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G196" sqref="G196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -5951,54 +5960,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:6">
       <c r="A204" t="s">
+        <v>482</v>
+      </c>
+      <c r="B204" t="s">
+        <v>483</v>
+      </c>
+      <c r="C204" t="s">
         <v>487</v>
       </c>
-      <c r="B204" t="s">
+      <c r="D204" t="s">
         <v>488</v>
       </c>
       <c r="E204">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:6">
+      <c r="F204" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B205" t="s">
-        <v>490</v>
-      </c>
-      <c r="C205" t="s">
         <v>491</v>
       </c>
-      <c r="D205" t="s">
+      <c r="E205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" t="s">
         <v>492</v>
       </c>
-      <c r="E205">
-        <v>0</v>
-      </c>
-      <c r="F205" t="s">
+      <c r="B206" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="206" spans="1:5">
-      <c r="A206" t="s">
+      <c r="C206" t="s">
         <v>494</v>
       </c>
-      <c r="B206" t="s">
+      <c r="D206" t="s">
         <v>495</v>
       </c>
       <c r="E206">
         <v>0</v>
+      </c>
+      <c r="F206" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="207" spans="1:5">
       <c r="A207" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B207" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E207">
         <v>0</v>
@@ -6006,10 +6024,10 @@
     </row>
     <row r="208" spans="1:5">
       <c r="A208" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B208" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E208">
         <v>0</v>
@@ -6017,16 +6035,10 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B209" t="s">
-        <v>501</v>
-      </c>
-      <c r="C209" t="s">
         <v>502</v>
-      </c>
-      <c r="D209" t="s">
-        <v>503</v>
       </c>
       <c r="E209">
         <v>0</v>
@@ -6034,10 +6046,16 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" t="s">
+        <v>503</v>
+      </c>
+      <c r="B210" t="s">
         <v>504</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>505</v>
+      </c>
+      <c r="D210" t="s">
+        <v>506</v>
       </c>
       <c r="E210">
         <v>0</v>
@@ -6045,38 +6063,38 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B211" t="s">
-        <v>507</v>
-      </c>
-      <c r="C211" t="s">
         <v>508</v>
       </c>
-      <c r="D211" t="s">
-        <v>509</v>
-      </c>
       <c r="E211">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:5">
       <c r="A212" t="s">
+        <v>509</v>
+      </c>
+      <c r="B212" t="s">
         <v>510</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212" t="s">
         <v>511</v>
       </c>
+      <c r="D212" t="s">
+        <v>512</v>
+      </c>
       <c r="E212">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:5">
       <c r="A213" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B213" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E213">
         <v>0</v>
@@ -6084,16 +6102,10 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B214" t="s">
-        <v>515</v>
-      </c>
-      <c r="C214" t="s">
         <v>516</v>
-      </c>
-      <c r="D214" t="s">
-        <v>517</v>
       </c>
       <c r="E214">
         <v>0</v>
@@ -6101,38 +6113,44 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="B215" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C215" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D215" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E215">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:5">
       <c r="A216" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B216" t="s">
+        <v>518</v>
+      </c>
+      <c r="C216" t="s">
         <v>521</v>
       </c>
+      <c r="D216" t="s">
+        <v>522</v>
+      </c>
       <c r="E216">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:5">
       <c r="A217" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B217" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E217">
         <v>0</v>
@@ -6140,10 +6158,10 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B218" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E218">
         <v>0</v>
@@ -6151,10 +6169,10 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B219" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E219">
         <v>0</v>
@@ -6162,10 +6180,10 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B220" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E220">
         <v>0</v>
@@ -6173,16 +6191,10 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B221" t="s">
-        <v>531</v>
-      </c>
-      <c r="C221" t="s">
         <v>532</v>
-      </c>
-      <c r="D221" t="s">
-        <v>533</v>
       </c>
       <c r="E221">
         <v>0</v>
@@ -6190,16 +6202,16 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B222" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C222" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D222" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E222">
         <v>0</v>
@@ -6207,16 +6219,16 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B223" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C223" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D223" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E223">
         <v>0</v>
@@ -6224,44 +6236,50 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B224" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C224" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D224" t="s">
-        <v>210</v>
+        <v>540</v>
       </c>
       <c r="E224">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:5">
       <c r="A225" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="B225" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="C225" t="s">
         <v>541</v>
       </c>
       <c r="D225" t="s">
-        <v>542</v>
+        <v>210</v>
       </c>
       <c r="E225">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:5">
       <c r="A226" t="s">
+        <v>542</v>
+      </c>
+      <c r="B226" t="s">
         <v>543</v>
       </c>
-      <c r="B226" t="s">
+      <c r="C226" t="s">
         <v>544</v>
+      </c>
+      <c r="D226" t="s">
+        <v>545</v>
       </c>
       <c r="E226">
         <v>0</v>
@@ -6269,10 +6287,10 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B227" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E227">
         <v>0</v>
@@ -6280,10 +6298,10 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B228" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E228">
         <v>0</v>
@@ -6291,10 +6309,10 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B229" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E229">
         <v>0</v>
@@ -6302,10 +6320,10 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B230" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E230">
         <v>0</v>
@@ -6313,10 +6331,10 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B231" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E231">
         <v>0</v>
@@ -6324,10 +6342,10 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B232" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E232">
         <v>0</v>
@@ -6335,10 +6353,10 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B233" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E233">
         <v>0</v>
@@ -6346,10 +6364,10 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B234" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E234">
         <v>0</v>
@@ -6357,10 +6375,10 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B235" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E235">
         <v>0</v>
@@ -6368,10 +6386,10 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B236" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E236">
         <v>0</v>
@@ -6379,16 +6397,10 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B237" t="s">
-        <v>566</v>
-      </c>
-      <c r="C237" t="s">
         <v>567</v>
-      </c>
-      <c r="D237" t="s">
-        <v>568</v>
       </c>
       <c r="E237">
         <v>0</v>
@@ -6396,10 +6408,16 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" t="s">
+        <v>568</v>
+      </c>
+      <c r="B238" t="s">
         <v>569</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>570</v>
+      </c>
+      <c r="D238" t="s">
+        <v>571</v>
       </c>
       <c r="E238">
         <v>0</v>
@@ -6407,10 +6425,10 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B239" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E239">
         <v>0</v>
@@ -6418,16 +6436,10 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B240" t="s">
-        <v>574</v>
-      </c>
-      <c r="C240" t="s">
         <v>575</v>
-      </c>
-      <c r="D240" t="s">
-        <v>576</v>
       </c>
       <c r="E240">
         <v>0</v>
@@ -6435,16 +6447,16 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" t="s">
+        <v>576</v>
+      </c>
+      <c r="B241" t="s">
         <v>577</v>
       </c>
-      <c r="B241" t="s">
+      <c r="C241" t="s">
         <v>578</v>
       </c>
-      <c r="C241" t="s">
+      <c r="D241" t="s">
         <v>579</v>
-      </c>
-      <c r="D241" t="s">
-        <v>580</v>
       </c>
       <c r="E241">
         <v>0</v>
@@ -6452,10 +6464,16 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" t="s">
+        <v>580</v>
+      </c>
+      <c r="B242" t="s">
         <v>581</v>
       </c>
-      <c r="B242" t="s">
+      <c r="C242" t="s">
         <v>582</v>
+      </c>
+      <c r="D242" t="s">
+        <v>583</v>
       </c>
       <c r="E242">
         <v>0</v>
@@ -6463,10 +6481,10 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B243" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E243">
         <v>0</v>
@@ -6474,10 +6492,10 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B244" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="E244">
         <v>0</v>
@@ -6485,10 +6503,10 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B245" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E245">
         <v>0</v>
@@ -6496,16 +6514,10 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B246" t="s">
-        <v>590</v>
-      </c>
-      <c r="C246" t="s">
         <v>591</v>
-      </c>
-      <c r="D246" t="s">
-        <v>592</v>
       </c>
       <c r="E246">
         <v>0</v>
@@ -6513,16 +6525,16 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="B247" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="C247" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D247" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="E247">
         <v>0</v>
@@ -6530,16 +6542,16 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B248" t="s">
+        <v>593</v>
+      </c>
+      <c r="C248" t="s">
         <v>596</v>
       </c>
-      <c r="C248" t="s">
+      <c r="D248" t="s">
         <v>597</v>
-      </c>
-      <c r="D248" t="s">
-        <v>598</v>
       </c>
       <c r="E248">
         <v>0</v>
@@ -6547,16 +6559,16 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="B249" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="C249" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D249" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="E249">
         <v>0</v>
@@ -6564,38 +6576,44 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="B250" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="C250" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D250" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="E250">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:5">
       <c r="A251" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="B251" t="s">
+        <v>599</v>
+      </c>
+      <c r="C251" t="s">
         <v>604</v>
       </c>
+      <c r="D251" t="s">
+        <v>605</v>
+      </c>
       <c r="E251">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:5">
       <c r="A252" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B252" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E252">
         <v>0</v>
@@ -6603,16 +6621,10 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B253" t="s">
-        <v>608</v>
-      </c>
-      <c r="C253" t="s">
         <v>609</v>
-      </c>
-      <c r="D253" t="s">
-        <v>610</v>
       </c>
       <c r="E253">
         <v>0</v>
@@ -6620,16 +6632,16 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" t="s">
+        <v>610</v>
+      </c>
+      <c r="B254" t="s">
         <v>611</v>
       </c>
-      <c r="B254" t="s">
+      <c r="C254" t="s">
         <v>612</v>
       </c>
-      <c r="C254" t="s">
+      <c r="D254" t="s">
         <v>613</v>
-      </c>
-      <c r="D254" t="s">
-        <v>614</v>
       </c>
       <c r="E254">
         <v>0</v>
@@ -6637,16 +6649,16 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B255" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C255" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D255" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E255">
         <v>0</v>
@@ -6654,16 +6666,16 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B256" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C256" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D256" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="E256">
         <v>0</v>
@@ -6671,16 +6683,16 @@
     </row>
     <row r="257" spans="1:5">
       <c r="A257" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B257" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C257" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D257" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="E257">
         <v>0</v>
@@ -6688,16 +6700,16 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B258" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C258" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D258" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E258">
         <v>0</v>
@@ -6705,16 +6717,16 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B259" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C259" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D259" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="E259">
         <v>0</v>
@@ -6722,10 +6734,16 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
       <c r="B260" t="s">
+        <v>615</v>
+      </c>
+      <c r="C260" t="s">
         <v>626</v>
+      </c>
+      <c r="D260" t="s">
+        <v>627</v>
       </c>
       <c r="E260">
         <v>0</v>
@@ -6733,16 +6751,10 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B261" t="s">
-        <v>628</v>
-      </c>
-      <c r="C261" t="s">
         <v>629</v>
-      </c>
-      <c r="D261" t="s">
-        <v>630</v>
       </c>
       <c r="E261">
         <v>0</v>
@@ -6750,10 +6762,16 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" t="s">
+        <v>630</v>
+      </c>
+      <c r="B262" t="s">
         <v>631</v>
       </c>
-      <c r="B262" t="s">
+      <c r="C262" t="s">
         <v>632</v>
+      </c>
+      <c r="D262" t="s">
+        <v>633</v>
       </c>
       <c r="E262">
         <v>0</v>
@@ -6761,10 +6779,10 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B263" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E263">
         <v>0</v>
@@ -6772,10 +6790,10 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B264" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E264">
         <v>0</v>
@@ -6783,16 +6801,10 @@
     </row>
     <row r="265" spans="1:5">
       <c r="A265" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B265" t="s">
-        <v>638</v>
-      </c>
-      <c r="C265" t="s">
         <v>639</v>
-      </c>
-      <c r="D265" t="s">
-        <v>640</v>
       </c>
       <c r="E265">
         <v>0</v>
@@ -6800,16 +6812,16 @@
     </row>
     <row r="266" spans="1:5">
       <c r="A266" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="B266" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="C266" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D266" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="E266">
         <v>0</v>
@@ -6817,16 +6829,16 @@
     </row>
     <row r="267" spans="1:5">
       <c r="A267" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B267" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C267" t="s">
         <v>644</v>
       </c>
       <c r="D267" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E267">
         <v>0</v>
@@ -6834,16 +6846,16 @@
     </row>
     <row r="268" spans="1:5">
       <c r="A268" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="B268" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="C268" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D268" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="E268">
         <v>0</v>
@@ -6851,16 +6863,16 @@
     </row>
     <row r="269" spans="1:5">
       <c r="A269" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="B269" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="C269" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D269" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="E269">
         <v>0</v>
@@ -6868,16 +6880,16 @@
     </row>
     <row r="270" spans="1:5">
       <c r="A270" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B270" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C270" t="s">
         <v>651</v>
       </c>
       <c r="D270" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="E270">
         <v>0</v>
@@ -6885,10 +6897,16 @@
     </row>
     <row r="271" spans="1:5">
       <c r="A271" t="s">
+        <v>652</v>
+      </c>
+      <c r="B271" t="s">
         <v>653</v>
       </c>
-      <c r="B271" t="s">
+      <c r="C271" t="s">
         <v>654</v>
+      </c>
+      <c r="D271" t="s">
+        <v>655</v>
       </c>
       <c r="E271">
         <v>0</v>
@@ -6896,10 +6914,10 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B272" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E272">
         <v>0</v>
@@ -6907,10 +6925,10 @@
     </row>
     <row r="273" spans="1:5">
       <c r="A273" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B273" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E273">
         <v>0</v>
@@ -6918,16 +6936,10 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B274" t="s">
-        <v>660</v>
-      </c>
-      <c r="C274" t="s">
         <v>661</v>
-      </c>
-      <c r="D274" t="s">
-        <v>662</v>
       </c>
       <c r="E274">
         <v>0</v>
@@ -6935,16 +6947,16 @@
     </row>
     <row r="275" spans="1:5">
       <c r="A275" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B275" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C275" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D275" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="E275">
         <v>0</v>
@@ -6952,13 +6964,13 @@
     </row>
     <row r="276" spans="1:5">
       <c r="A276" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B276" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C276" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="D276" t="s">
         <v>665</v>
@@ -6969,10 +6981,16 @@
     </row>
     <row r="277" spans="1:5">
       <c r="A277" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B277" t="s">
+        <v>663</v>
+      </c>
+      <c r="C277" t="s">
         <v>667</v>
+      </c>
+      <c r="D277" t="s">
+        <v>668</v>
       </c>
       <c r="E277">
         <v>0</v>
@@ -6980,10 +6998,10 @@
     </row>
     <row r="278" spans="1:5">
       <c r="A278" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B278" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E278">
         <v>0</v>
@@ -6991,10 +7009,10 @@
     </row>
     <row r="279" spans="1:5">
       <c r="A279" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B279" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E279">
         <v>0</v>
@@ -7002,10 +7020,10 @@
     </row>
     <row r="280" spans="1:5">
       <c r="A280" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B280" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E280">
         <v>0</v>
@@ -7013,44 +7031,38 @@
     </row>
     <row r="281" spans="1:5">
       <c r="A281" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B281" t="s">
-        <v>675</v>
-      </c>
-      <c r="C281" t="s">
         <v>676</v>
       </c>
-      <c r="D281" t="s">
-        <v>677</v>
-      </c>
       <c r="E281">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:5">
       <c r="A282" t="s">
+        <v>677</v>
+      </c>
+      <c r="B282" t="s">
         <v>678</v>
       </c>
-      <c r="B282" t="s">
+      <c r="C282" t="s">
         <v>679</v>
       </c>
+      <c r="D282" t="s">
+        <v>680</v>
+      </c>
       <c r="E282">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283" spans="1:5">
       <c r="A283" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B283" t="s">
-        <v>681</v>
-      </c>
-      <c r="C283" t="s">
         <v>682</v>
-      </c>
-      <c r="D283" t="s">
-        <v>683</v>
       </c>
       <c r="E283">
         <v>0</v>
@@ -7058,16 +7070,16 @@
     </row>
     <row r="284" spans="1:5">
       <c r="A284" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="B284" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="C284" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D284" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E284">
         <v>0</v>
@@ -7075,10 +7087,16 @@
     </row>
     <row r="285" spans="1:5">
       <c r="A285" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B285" t="s">
+        <v>684</v>
+      </c>
+      <c r="C285" t="s">
         <v>687</v>
+      </c>
+      <c r="D285" t="s">
+        <v>688</v>
       </c>
       <c r="E285">
         <v>0</v>
@@ -7086,10 +7104,10 @@
     </row>
     <row r="286" spans="1:5">
       <c r="A286" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B286" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E286">
         <v>0</v>
@@ -7097,10 +7115,10 @@
     </row>
     <row r="287" spans="1:5">
       <c r="A287" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B287" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="E287">
         <v>0</v>
@@ -7108,10 +7126,10 @@
     </row>
     <row r="288" spans="1:5">
       <c r="A288" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B288" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E288">
         <v>0</v>
@@ -7119,10 +7137,10 @@
     </row>
     <row r="289" spans="1:5">
       <c r="A289" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B289" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="E289">
         <v>0</v>
@@ -7130,44 +7148,44 @@
     </row>
     <row r="290" spans="1:5">
       <c r="A290" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B290" t="s">
-        <v>697</v>
-      </c>
-      <c r="C290" t="s">
         <v>698</v>
       </c>
-      <c r="D290" t="s">
-        <v>699</v>
-      </c>
       <c r="E290">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291" spans="1:5">
       <c r="A291" t="s">
+        <v>699</v>
+      </c>
+      <c r="B291" t="s">
         <v>700</v>
       </c>
-      <c r="B291" t="s">
+      <c r="C291" t="s">
         <v>701</v>
       </c>
-      <c r="C291" t="s">
+      <c r="D291" t="s">
         <v>702</v>
       </c>
-      <c r="D291" t="s">
-        <v>703</v>
-      </c>
       <c r="E291">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292" spans="1:5">
       <c r="A292" t="s">
+        <v>703</v>
+      </c>
+      <c r="B292" t="s">
         <v>704</v>
       </c>
-      <c r="B292" t="s">
+      <c r="C292" t="s">
         <v>705</v>
+      </c>
+      <c r="D292" t="s">
+        <v>706</v>
       </c>
       <c r="E292">
         <v>0</v>
@@ -7175,10 +7193,10 @@
     </row>
     <row r="293" spans="1:5">
       <c r="A293" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B293" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="E293">
         <v>0</v>
@@ -7186,33 +7204,27 @@
     </row>
     <row r="294" spans="1:5">
       <c r="A294" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B294" t="s">
-        <v>709</v>
-      </c>
-      <c r="C294" t="s">
         <v>710</v>
       </c>
-      <c r="D294" t="s">
-        <v>711</v>
-      </c>
       <c r="E294">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:5">
       <c r="A295" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B295" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="C295" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D295" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E295">
         <v>1</v>
@@ -7220,16 +7232,16 @@
     </row>
     <row r="296" spans="1:5">
       <c r="A296" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B296" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="C296" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D296" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E296">
         <v>1</v>
@@ -7237,16 +7249,16 @@
     </row>
     <row r="297" spans="1:5">
       <c r="A297" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B297" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="C297" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D297" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="E297">
         <v>1</v>
@@ -7254,21 +7266,27 @@
     </row>
     <row r="298" spans="1:5">
       <c r="A298" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
       <c r="B298" t="s">
+        <v>712</v>
+      </c>
+      <c r="C298" t="s">
         <v>719</v>
       </c>
+      <c r="D298" t="s">
+        <v>720</v>
+      </c>
       <c r="E298">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:5">
       <c r="A299" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B299" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="E299">
         <v>0</v>
@@ -7276,10 +7294,10 @@
     </row>
     <row r="300" spans="1:5">
       <c r="A300" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B300" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E300">
         <v>0</v>
@@ -7287,10 +7305,10 @@
     </row>
     <row r="301" spans="1:5">
       <c r="A301" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B301" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E301">
         <v>0</v>
@@ -7298,52 +7316,52 @@
     </row>
     <row r="302" spans="1:5">
       <c r="A302" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B302" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="E302">
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:6">
+    <row r="303" spans="1:5">
       <c r="A303" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B303" t="s">
-        <v>729</v>
-      </c>
-      <c r="C303" t="s">
         <v>730</v>
       </c>
-      <c r="D303" t="s">
+      <c r="E303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6">
+      <c r="A304" t="s">
         <v>731</v>
       </c>
-      <c r="E303">
+      <c r="B304" t="s">
+        <v>732</v>
+      </c>
+      <c r="C304" t="s">
+        <v>733</v>
+      </c>
+      <c r="D304" t="s">
+        <v>734</v>
+      </c>
+      <c r="E304">
         <v>1</v>
       </c>
-      <c r="F303" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="304" spans="1:5">
-      <c r="A304" t="s">
-        <v>733</v>
-      </c>
-      <c r="B304" t="s">
-        <v>734</v>
-      </c>
-      <c r="E304">
-        <v>0</v>
+      <c r="F304" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="305" spans="1:5">
       <c r="A305" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B305" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="E305">
         <v>0</v>
@@ -7351,10 +7369,10 @@
     </row>
     <row r="306" spans="1:5">
       <c r="A306" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B306" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="E306">
         <v>0</v>
@@ -7362,10 +7380,10 @@
     </row>
     <row r="307" spans="1:5">
       <c r="A307" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B307" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E307">
         <v>0</v>
@@ -7373,16 +7391,10 @@
     </row>
     <row r="308" spans="1:5">
       <c r="A308" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B308" t="s">
-        <v>742</v>
-      </c>
-      <c r="C308" t="s">
         <v>743</v>
-      </c>
-      <c r="D308" t="s">
-        <v>744</v>
       </c>
       <c r="E308">
         <v>0</v>
@@ -7390,16 +7402,16 @@
     </row>
     <row r="309" spans="1:5">
       <c r="A309" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="B309" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="C309" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D309" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E309">
         <v>0</v>
@@ -7407,16 +7419,16 @@
     </row>
     <row r="310" spans="1:5">
       <c r="A310" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="B310" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="C310" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="D310" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="E310">
         <v>0</v>
@@ -7424,18 +7436,35 @@
     </row>
     <row r="311" spans="1:5">
       <c r="A311" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="B311" t="s">
+        <v>745</v>
+      </c>
+      <c r="C311" t="s">
         <v>750</v>
       </c>
+      <c r="D311" t="s">
+        <v>751</v>
+      </c>
       <c r="E311">
         <v>0</v>
       </c>
     </row>
+    <row r="312" spans="1:5">
+      <c r="A312" t="s">
+        <v>752</v>
+      </c>
+      <c r="B312" t="s">
+        <v>753</v>
+      </c>
+      <c r="E312">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F311">
-    <sortState ref="A2:F311">
+  <autoFilter ref="A1:F312">
+    <sortState ref="A2:F312">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
working D3 example, via: http://bl.ocks.org/micahstubbs/8e15870eb432a21f0bc4d3d527b2d14f / https://gist.github.com/micahstubbs/8e15870eb432a21f0bc4d3d527b2d14f (mentions CC0-1.0 license)
</commit_message>
<xml_diff>
--- a/read_the_world.xlsx
+++ b/read_the_world.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$314</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$315</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760">
   <si>
     <t>Code</t>
   </si>
@@ -1847,6 +1847,12 @@
   </si>
   <si>
     <t>Trevor Noah</t>
+  </si>
+  <si>
+    <t>Long Walk to Freedom</t>
+  </si>
+  <si>
+    <t>Nelson Mandela</t>
   </si>
   <si>
     <t>GS</t>
@@ -3237,12 +3243,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G314"/>
+  <dimension ref="A1:G315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="I249" sqref="I249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -6656,9 +6662,15 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" t="s">
+        <v>602</v>
+      </c>
+      <c r="B254" t="s">
+        <v>603</v>
+      </c>
+      <c r="C254" t="s">
         <v>610</v>
       </c>
-      <c r="B254" t="s">
+      <c r="D254" t="s">
         <v>611</v>
       </c>
       <c r="E254">
@@ -6683,28 +6695,22 @@
       <c r="B256" t="s">
         <v>615</v>
       </c>
-      <c r="C256" t="s">
-        <v>616</v>
-      </c>
-      <c r="D256" t="s">
-        <v>617</v>
-      </c>
       <c r="E256">
         <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:5">
       <c r="A257" t="s">
+        <v>616</v>
+      </c>
+      <c r="B257" t="s">
+        <v>617</v>
+      </c>
+      <c r="C257" t="s">
         <v>618</v>
       </c>
-      <c r="B257" t="s">
+      <c r="D257" t="s">
         <v>619</v>
-      </c>
-      <c r="C257" t="s">
-        <v>620</v>
-      </c>
-      <c r="D257" t="s">
-        <v>621</v>
       </c>
       <c r="E257">
         <v>0</v>
@@ -6712,10 +6718,10 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B258" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C258" t="s">
         <v>622</v>
@@ -6729,10 +6735,10 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B259" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C259" t="s">
         <v>624</v>
@@ -6746,10 +6752,10 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B260" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C260" t="s">
         <v>626</v>
@@ -6763,10 +6769,10 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B261" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C261" t="s">
         <v>628</v>
@@ -6780,10 +6786,10 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B262" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C262" t="s">
         <v>630</v>
@@ -6797,9 +6803,15 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" t="s">
+        <v>620</v>
+      </c>
+      <c r="B263" t="s">
+        <v>621</v>
+      </c>
+      <c r="C263" t="s">
         <v>632</v>
       </c>
-      <c r="B263" t="s">
+      <c r="D263" t="s">
         <v>633</v>
       </c>
       <c r="E263">
@@ -6813,21 +6825,21 @@
       <c r="B264" t="s">
         <v>635</v>
       </c>
-      <c r="C264" t="s">
-        <v>636</v>
-      </c>
-      <c r="D264" t="s">
-        <v>637</v>
-      </c>
       <c r="E264">
         <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:5">
       <c r="A265" t="s">
+        <v>636</v>
+      </c>
+      <c r="B265" t="s">
+        <v>637</v>
+      </c>
+      <c r="C265" t="s">
         <v>638</v>
       </c>
-      <c r="B265" t="s">
+      <c r="D265" t="s">
         <v>639</v>
       </c>
       <c r="E265">
@@ -6863,28 +6875,22 @@
       <c r="B268" t="s">
         <v>645</v>
       </c>
-      <c r="C268" t="s">
-        <v>646</v>
-      </c>
-      <c r="D268" t="s">
-        <v>647</v>
-      </c>
       <c r="E268">
         <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:5">
       <c r="A269" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="B269" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="C269" t="s">
         <v>648</v>
       </c>
       <c r="D269" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="E269">
         <v>0</v>
@@ -6892,16 +6898,16 @@
     </row>
     <row r="270" spans="1:5">
       <c r="A270" t="s">
+        <v>646</v>
+      </c>
+      <c r="B270" t="s">
+        <v>647</v>
+      </c>
+      <c r="C270" t="s">
+        <v>650</v>
+      </c>
+      <c r="D270" t="s">
         <v>649</v>
-      </c>
-      <c r="B270" t="s">
-        <v>650</v>
-      </c>
-      <c r="C270" t="s">
-        <v>651</v>
-      </c>
-      <c r="D270" t="s">
-        <v>652</v>
       </c>
       <c r="E270">
         <v>0</v>
@@ -6909,10 +6915,10 @@
     </row>
     <row r="271" spans="1:5">
       <c r="A271" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B271" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="C271" t="s">
         <v>653</v>
@@ -6926,16 +6932,16 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B272" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="C272" t="s">
         <v>655</v>
       </c>
       <c r="D272" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="E272">
         <v>0</v>
@@ -6943,16 +6949,16 @@
     </row>
     <row r="273" spans="1:5">
       <c r="A273" t="s">
+        <v>651</v>
+      </c>
+      <c r="B273" t="s">
+        <v>652</v>
+      </c>
+      <c r="C273" t="s">
+        <v>657</v>
+      </c>
+      <c r="D273" t="s">
         <v>656</v>
-      </c>
-      <c r="B273" t="s">
-        <v>657</v>
-      </c>
-      <c r="C273" t="s">
-        <v>658</v>
-      </c>
-      <c r="D273" t="s">
-        <v>659</v>
       </c>
       <c r="E273">
         <v>0</v>
@@ -6960,9 +6966,15 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" t="s">
+        <v>658</v>
+      </c>
+      <c r="B274" t="s">
+        <v>659</v>
+      </c>
+      <c r="C274" t="s">
         <v>660</v>
       </c>
-      <c r="B274" t="s">
+      <c r="D274" t="s">
         <v>661</v>
       </c>
       <c r="E274">
@@ -6998,28 +7010,22 @@
       <c r="B277" t="s">
         <v>667</v>
       </c>
-      <c r="C277" t="s">
-        <v>668</v>
-      </c>
-      <c r="D277" t="s">
-        <v>669</v>
-      </c>
       <c r="E277">
         <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:5">
       <c r="A278" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B278" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C278" t="s">
         <v>670</v>
       </c>
       <c r="D278" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="E278">
         <v>0</v>
@@ -7027,16 +7033,16 @@
     </row>
     <row r="279" spans="1:5">
       <c r="A279" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B279" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="C279" t="s">
+        <v>672</v>
+      </c>
+      <c r="D279" t="s">
         <v>671</v>
-      </c>
-      <c r="D279" t="s">
-        <v>672</v>
       </c>
       <c r="E279">
         <v>0</v>
@@ -7044,9 +7050,15 @@
     </row>
     <row r="280" spans="1:5">
       <c r="A280" t="s">
+        <v>668</v>
+      </c>
+      <c r="B280" t="s">
+        <v>669</v>
+      </c>
+      <c r="C280" t="s">
         <v>673</v>
       </c>
-      <c r="B280" t="s">
+      <c r="D280" t="s">
         <v>674</v>
       </c>
       <c r="E280">
@@ -7093,25 +7105,25 @@
       <c r="B284" t="s">
         <v>682</v>
       </c>
-      <c r="C284" t="s">
-        <v>683</v>
-      </c>
-      <c r="D284" t="s">
-        <v>684</v>
-      </c>
       <c r="E284">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285" spans="1:5">
       <c r="A285" t="s">
+        <v>683</v>
+      </c>
+      <c r="B285" t="s">
+        <v>684</v>
+      </c>
+      <c r="C285" t="s">
         <v>685</v>
       </c>
-      <c r="B285" t="s">
+      <c r="D285" t="s">
         <v>686</v>
       </c>
       <c r="E285">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -7121,22 +7133,16 @@
       <c r="B286" t="s">
         <v>688</v>
       </c>
-      <c r="C286" t="s">
-        <v>689</v>
-      </c>
-      <c r="D286" t="s">
-        <v>690</v>
-      </c>
       <c r="E286">
         <v>0</v>
       </c>
     </row>
     <row r="287" spans="1:5">
       <c r="A287" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="B287" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="C287" t="s">
         <v>691</v>
@@ -7150,9 +7156,15 @@
     </row>
     <row r="288" spans="1:5">
       <c r="A288" t="s">
+        <v>689</v>
+      </c>
+      <c r="B288" t="s">
+        <v>690</v>
+      </c>
+      <c r="C288" t="s">
         <v>693</v>
       </c>
-      <c r="B288" t="s">
+      <c r="D288" t="s">
         <v>694</v>
       </c>
       <c r="E288">
@@ -7210,38 +7222,38 @@
       <c r="B293" t="s">
         <v>704</v>
       </c>
-      <c r="C293" t="s">
-        <v>705</v>
-      </c>
-      <c r="D293" t="s">
-        <v>706</v>
-      </c>
       <c r="E293">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294" spans="1:5">
       <c r="A294" t="s">
+        <v>705</v>
+      </c>
+      <c r="B294" t="s">
+        <v>706</v>
+      </c>
+      <c r="C294" t="s">
         <v>707</v>
       </c>
-      <c r="B294" t="s">
+      <c r="D294" t="s">
         <v>708</v>
       </c>
-      <c r="C294" t="s">
-        <v>709</v>
-      </c>
-      <c r="D294" t="s">
-        <v>710</v>
-      </c>
       <c r="E294">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:5">
       <c r="A295" t="s">
+        <v>709</v>
+      </c>
+      <c r="B295" t="s">
+        <v>710</v>
+      </c>
+      <c r="C295" t="s">
         <v>711</v>
       </c>
-      <c r="B295" t="s">
+      <c r="D295" t="s">
         <v>712</v>
       </c>
       <c r="E295">
@@ -7266,22 +7278,16 @@
       <c r="B297" t="s">
         <v>716</v>
       </c>
-      <c r="C297" t="s">
-        <v>717</v>
-      </c>
-      <c r="D297" t="s">
-        <v>718</v>
-      </c>
       <c r="E297">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:5">
       <c r="A298" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B298" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C298" t="s">
         <v>719</v>
@@ -7295,10 +7301,10 @@
     </row>
     <row r="299" spans="1:5">
       <c r="A299" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B299" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C299" t="s">
         <v>721</v>
@@ -7312,10 +7318,10 @@
     </row>
     <row r="300" spans="1:5">
       <c r="A300" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B300" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C300" t="s">
         <v>723</v>
@@ -7329,13 +7335,19 @@
     </row>
     <row r="301" spans="1:5">
       <c r="A301" t="s">
+        <v>717</v>
+      </c>
+      <c r="B301" t="s">
+        <v>718</v>
+      </c>
+      <c r="C301" t="s">
         <v>725</v>
       </c>
-      <c r="B301" t="s">
+      <c r="D301" t="s">
         <v>726</v>
       </c>
       <c r="E301">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302" spans="1:5">
@@ -7382,35 +7394,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:6">
+    <row r="306" spans="1:5">
       <c r="A306" t="s">
         <v>735</v>
       </c>
       <c r="B306" t="s">
         <v>736</v>
       </c>
-      <c r="C306" t="s">
+      <c r="E306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6">
+      <c r="A307" t="s">
         <v>737</v>
       </c>
-      <c r="D306" t="s">
+      <c r="B307" t="s">
         <v>738</v>
       </c>
-      <c r="E306">
+      <c r="C307" t="s">
+        <v>739</v>
+      </c>
+      <c r="D307" t="s">
+        <v>740</v>
+      </c>
+      <c r="E307">
         <v>1</v>
       </c>
-      <c r="F306" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="307" spans="1:5">
-      <c r="A307" t="s">
-        <v>740</v>
-      </c>
-      <c r="B307" t="s">
+      <c r="F307" t="s">
         <v>741</v>
-      </c>
-      <c r="E307">
-        <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -7453,22 +7465,16 @@
       <c r="B311" t="s">
         <v>749</v>
       </c>
-      <c r="C311" t="s">
-        <v>750</v>
-      </c>
-      <c r="D311" t="s">
-        <v>751</v>
-      </c>
       <c r="E311">
         <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:5">
       <c r="A312" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B312" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="C312" t="s">
         <v>752</v>
@@ -7482,10 +7488,10 @@
     </row>
     <row r="313" spans="1:5">
       <c r="A313" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="B313" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="C313" t="s">
         <v>754</v>
@@ -7499,18 +7505,35 @@
     </row>
     <row r="314" spans="1:5">
       <c r="A314" t="s">
+        <v>750</v>
+      </c>
+      <c r="B314" t="s">
+        <v>751</v>
+      </c>
+      <c r="C314" t="s">
         <v>756</v>
       </c>
-      <c r="B314" t="s">
+      <c r="D314" t="s">
         <v>757</v>
       </c>
       <c r="E314">
         <v>0</v>
       </c>
     </row>
+    <row r="315" spans="1:5">
+      <c r="A315" t="s">
+        <v>758</v>
+      </c>
+      <c r="B315" t="s">
+        <v>759</v>
+      </c>
+      <c r="E315">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F314">
-    <sortState ref="A1:F314">
+  <autoFilter ref="A1:F315">
+    <sortState ref="A1:F315">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>